<commit_message>
editing plots & adding SQL queries
</commit_message>
<xml_diff>
--- a/data/processed/treatment_group_final.xlsx
+++ b/data/processed/treatment_group_final.xlsx
@@ -1,374 +1,382 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulsharratt/Documents/Hertie/Semester 4/03 - Master's Thesis/thesis_stf/data/processed/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC195243-88B9-B949-9896-6FF7E0B4637E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="17540" yWindow="2120" windowWidth="17680" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
-  <si>
-    <t xml:space="preserve">org</t>
-  </si>
-  <si>
-    <t xml:space="preserve">repo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">org_url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">repo_url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">repo_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contracting_entity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">volume</t>
-  </si>
-  <si>
-    <t xml:space="preserve">start_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">end_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">apache</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logging-log4j2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/apache/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/apache/logging-log4j2/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grobmeier Solutions (Log4j)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">curl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/curl/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/curl/curl/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WolfSSL (curl (Daniel Stenberg))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fortran-lang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fpm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/fortran-lang/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/fortran-lang/fpm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NumFocus (Fortran)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NumFocus (Fortran (2023))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GNOME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">libxml2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/GNOME/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/GNOME/libxml2/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aevum GmbH (libxml2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GStreamer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qt-gstreamer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/GStreamer/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/GStreamer/qt-gstreamer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centricular Ltd (Gstreamer RTP)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lullabot</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drupal9ci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Lullabot/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/Lullabot/drupal9ci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drupal Association (Drupal (2023))</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLnetLabs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">domain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/NLnetLabs/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/NLnetLabs/domain/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NLNet Labs (domain)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">openjs-foundation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/openjs-foundation/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpenJS Foundation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpenMathLib</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpenBLAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/OpenMathLib/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/OpenMathLib/OpenBLAS/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OpenTeams (OpenBLAS)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">openmls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/openmls/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/openmls/openmls</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="118">
+  <si>
+    <t>org</t>
+  </si>
+  <si>
+    <t>repo</t>
+  </si>
+  <si>
+    <t>org_url</t>
+  </si>
+  <si>
+    <t>repo_url</t>
+  </si>
+  <si>
+    <t>repo_id</t>
+  </si>
+  <si>
+    <t>contracting_entity</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
+  </si>
+  <si>
+    <t>apache</t>
+  </si>
+  <si>
+    <t>logging-log4j2</t>
+  </si>
+  <si>
+    <t>https://github.com/apache/</t>
+  </si>
+  <si>
+    <t>https://github.com/apache/logging-log4j2/</t>
+  </si>
+  <si>
+    <t>Grobmeier Solutions (Log4j)</t>
+  </si>
+  <si>
+    <t>curl</t>
+  </si>
+  <si>
+    <t>https://github.com/curl/</t>
+  </si>
+  <si>
+    <t>https://github.com/curl/curl/</t>
+  </si>
+  <si>
+    <t>WolfSSL (curl (Daniel Stenberg))</t>
+  </si>
+  <si>
+    <t>fortran-lang</t>
+  </si>
+  <si>
+    <t>fpm</t>
+  </si>
+  <si>
+    <t>https://github.com/fortran-lang/</t>
+  </si>
+  <si>
+    <t>https://github.com/fortran-lang/fpm</t>
+  </si>
+  <si>
+    <t>NumFocus (Fortran)</t>
+  </si>
+  <si>
+    <t>NumFocus (Fortran (2023))</t>
+  </si>
+  <si>
+    <t>GNOME</t>
+  </si>
+  <si>
+    <t>libxml2</t>
+  </si>
+  <si>
+    <t>https://github.com/GNOME/</t>
+  </si>
+  <si>
+    <t>https://github.com/GNOME/libxml2/</t>
+  </si>
+  <si>
+    <t>aevum GmbH (libxml2)</t>
+  </si>
+  <si>
+    <t>GStreamer</t>
+  </si>
+  <si>
+    <t>qt-gstreamer</t>
+  </si>
+  <si>
+    <t>https://github.com/GStreamer/</t>
+  </si>
+  <si>
+    <t>https://github.com/GStreamer/qt-gstreamer</t>
+  </si>
+  <si>
+    <t>Centricular Ltd (Gstreamer RTP)</t>
+  </si>
+  <si>
+    <t>Lullabot</t>
+  </si>
+  <si>
+    <t>drupal9ci</t>
+  </si>
+  <si>
+    <t>https://github.com/Lullabot/</t>
+  </si>
+  <si>
+    <t>https://github.com/Lullabot/drupal9ci</t>
+  </si>
+  <si>
+    <t>Drupal Association (Drupal (2023))</t>
+  </si>
+  <si>
+    <t>NLnetLabs</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>https://github.com/NLnetLabs/</t>
+  </si>
+  <si>
+    <t>https://github.com/NLnetLabs/domain/</t>
+  </si>
+  <si>
+    <t>NLNet Labs (domain)</t>
+  </si>
+  <si>
+    <t>openjs-foundation</t>
+  </si>
+  <si>
+    <t>https://github.com/openjs-foundation/</t>
+  </si>
+  <si>
+    <t>OpenJS Foundation</t>
+  </si>
+  <si>
+    <t>OpenMathLib</t>
+  </si>
+  <si>
+    <t>OpenBLAS</t>
+  </si>
+  <si>
+    <t>https://github.com/OpenMathLib/</t>
+  </si>
+  <si>
+    <t>https://github.com/OpenMathLib/OpenBLAS/</t>
+  </si>
+  <si>
+    <t>OpenTeams (OpenBLAS)</t>
+  </si>
+  <si>
+    <t>openmls</t>
+  </si>
+  <si>
+    <t>https://github.com/openmls/</t>
+  </si>
+  <si>
+    <t>https://github.com/openmls/openmls</t>
   </si>
   <si>
     <t xml:space="preserve">Phoenix R&amp;D GmbH (OpenMLS (Raphael))
 </t>
   </si>
   <si>
-    <t xml:space="preserve">openpgpjs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/openpgpjs/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/openpgpjs/openpgpjs/</t>
+    <t>openpgpjs</t>
+  </si>
+  <si>
+    <t>https://github.com/openpgpjs/</t>
+  </si>
+  <si>
+    <t>https://github.com/openpgpjs/openpgpjs/</t>
   </si>
   <si>
     <t xml:space="preserve">Proton AG (OpenPGP.js (Daniel))
 </t>
   </si>
   <si>
-    <t xml:space="preserve">pendulum-project</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ntpd-rs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/pendulum-project/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/pendulum-project/ntpd-rs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TweedeGolf (Pendulum)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">web-pecl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/php/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/php/web-pecl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Open Source Collective (PHP Ecosystem)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prefix-dev</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rattler-build</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/prefix-dev/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/prefix-dev/rattler-build</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://prefix.dev GmbH (mamba)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pyca</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cryptography</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/pyca/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/pyca/cryptography/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trail of Bits (PyPi_Sigstore)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qos-ch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">logback</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/qos-ch/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/qos-ch/logback</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QOS.ch Sárl (logback)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rubygems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/rubygems/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/rubygems/rubygems</t>
+    <t>pendulum-project</t>
+  </si>
+  <si>
+    <t>ntpd-rs</t>
+  </si>
+  <si>
+    <t>https://github.com/pendulum-project/</t>
+  </si>
+  <si>
+    <t>https://github.com/pendulum-project/ntpd-rs</t>
+  </si>
+  <si>
+    <t>TweedeGolf (Pendulum)</t>
+  </si>
+  <si>
+    <t>php</t>
+  </si>
+  <si>
+    <t>web-pecl</t>
+  </si>
+  <si>
+    <t>https://github.com/php/</t>
+  </si>
+  <si>
+    <t>https://github.com/php/web-pecl</t>
+  </si>
+  <si>
+    <t>Open Source Collective (PHP Ecosystem)</t>
+  </si>
+  <si>
+    <t>prefix-dev</t>
+  </si>
+  <si>
+    <t>rattler-build</t>
+  </si>
+  <si>
+    <t>https://github.com/prefix-dev/</t>
+  </si>
+  <si>
+    <t>https://github.com/prefix-dev/rattler-build</t>
+  </si>
+  <si>
+    <t>http://prefix.dev GmbH (mamba)</t>
+  </si>
+  <si>
+    <t>pyca</t>
+  </si>
+  <si>
+    <t>cryptography</t>
+  </si>
+  <si>
+    <t>https://github.com/pyca/</t>
+  </si>
+  <si>
+    <t>https://github.com/pyca/cryptography/</t>
+  </si>
+  <si>
+    <t>Trail of Bits (PyPi_Sigstore)</t>
+  </si>
+  <si>
+    <t>qos-ch</t>
+  </si>
+  <si>
+    <t>logback</t>
+  </si>
+  <si>
+    <t>https://github.com/qos-ch/</t>
+  </si>
+  <si>
+    <t>https://github.com/qos-ch/logback</t>
+  </si>
+  <si>
+    <t>QOS.ch Sárl (logback)</t>
+  </si>
+  <si>
+    <t>rubygems</t>
+  </si>
+  <si>
+    <t>https://github.com/rubygems/</t>
+  </si>
+  <si>
+    <t>https://github.com/rubygems/rubygems</t>
   </si>
   <si>
     <t xml:space="preserve">Ruby Central Inc. (RubyGems &amp; Bundler (André))
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Ruby Central Inc. (RubyGems 2023)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rustls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/rustls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/rustls/rustls</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ISRG (Prossimo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">systemd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/systemd/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/systemd/systemd/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Codethink (systemd)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tc39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/tc39/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/tc39/test262</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Igalia S. L. (Web Development Libraries)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uutils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coreutils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/uutils/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/uutils/coreutils</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Les Bonnes Resolutions (Debian Rust/Coreutils)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">w3c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activitypub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/w3c/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/w3c/activitypub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">learningProof AG (activity pub)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequoia-pgp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fast-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/sequoia-pgp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://github.com/sequoia-pgp/fast-forward</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pibit AG (Sequoia PGP)</t>
+    <t>Ruby Central Inc. (RubyGems 2023)</t>
+  </si>
+  <si>
+    <t>rustls</t>
+  </si>
+  <si>
+    <t>https://github.com/rustls</t>
+  </si>
+  <si>
+    <t>https://github.com/rustls/rustls</t>
+  </si>
+  <si>
+    <t>ISRG (Prossimo)</t>
+  </si>
+  <si>
+    <t>systemd</t>
+  </si>
+  <si>
+    <t>https://github.com/systemd/</t>
+  </si>
+  <si>
+    <t>https://github.com/systemd/systemd/</t>
+  </si>
+  <si>
+    <t>Codethink (systemd)</t>
+  </si>
+  <si>
+    <t>tc39</t>
+  </si>
+  <si>
+    <t>test262</t>
+  </si>
+  <si>
+    <t>https://github.com/tc39/</t>
+  </si>
+  <si>
+    <t>https://github.com/tc39/test262</t>
+  </si>
+  <si>
+    <t>Igalia S. L. (Web Development Libraries)</t>
+  </si>
+  <si>
+    <t>uutils</t>
+  </si>
+  <si>
+    <t>coreutils</t>
+  </si>
+  <si>
+    <t>https://github.com/uutils/</t>
+  </si>
+  <si>
+    <t>https://github.com/uutils/coreutils</t>
+  </si>
+  <si>
+    <t>Les Bonnes Resolutions (Debian Rust/Coreutils)</t>
+  </si>
+  <si>
+    <t>w3c</t>
+  </si>
+  <si>
+    <t>activitypub</t>
+  </si>
+  <si>
+    <t>https://github.com/w3c/</t>
+  </si>
+  <si>
+    <t>https://github.com/w3c/activitypub</t>
+  </si>
+  <si>
+    <t>learningProof AG (activity pub)</t>
+  </si>
+  <si>
+    <t>sequoia-pgp</t>
+  </si>
+  <si>
+    <t>fast-forward</t>
+  </si>
+  <si>
+    <t>https://github.com/sequoia-pgp</t>
+  </si>
+  <si>
+    <t>https://github.com/sequoia-pgp/fast-forward</t>
+  </si>
+  <si>
+    <t>Pibit AG (Sequoia PGP)</t>
   </si>
 </sst>
 </file>
@@ -376,9 +384,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -390,6 +398,15 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -409,17 +426,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -701,14 +730,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="41.5" customWidth="1"/>
+    <col min="4" max="4" width="44.5" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" customWidth="1"/>
+    <col min="9" max="9" width="27.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -737,7 +775,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -750,23 +788,23 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>37405</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>596160</v>
       </c>
-      <c r="H2" s="1" t="n">
+      <c r="H2" s="1">
         <v>45149</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -779,23 +817,23 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3">
         <v>193661</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3">
         <v>195000</v>
       </c>
-      <c r="H3" s="1" t="n">
+      <c r="H3" s="1">
         <v>44855</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I3" s="1">
         <v>45067</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -808,23 +846,23 @@
       <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4">
         <v>191494</v>
       </c>
       <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4">
         <v>200000</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="H4" s="1">
         <v>44875</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="I4" s="1">
         <v>45087</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -837,23 +875,23 @@
       <c r="D5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5">
         <v>191494</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5">
         <v>612000</v>
       </c>
-      <c r="H5" s="1" t="n">
+      <c r="H5" s="1">
         <v>45124</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -866,23 +904,23 @@
       <c r="D6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6">
         <v>150821</v>
       </c>
       <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6">
         <v>136000</v>
       </c>
-      <c r="H6" s="1" t="n">
+      <c r="H6" s="1">
         <v>45141</v>
       </c>
-      <c r="I6" s="1" t="n">
+      <c r="I6" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -892,26 +930,26 @@
       <c r="C7" t="s">
         <v>31</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>151274</v>
       </c>
       <c r="F7" t="s">
         <v>33</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7">
         <v>203000</v>
       </c>
-      <c r="H7" s="1" t="n">
+      <c r="H7" s="1">
         <v>45201</v>
       </c>
-      <c r="I7" s="1" t="n">
+      <c r="I7" s="1">
         <v>45291</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -921,26 +959,26 @@
       <c r="C8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8">
         <v>150985</v>
       </c>
       <c r="F8" t="s">
         <v>38</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8">
         <v>278700</v>
       </c>
-      <c r="H8" s="1" t="n">
+      <c r="H8" s="1">
         <v>45201</v>
       </c>
-      <c r="I8" s="1" t="n">
+      <c r="I8" s="1">
         <v>45291</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -953,48 +991,46 @@
       <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9">
         <v>150832</v>
       </c>
       <c r="F9" t="s">
         <v>43</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9">
         <v>993600</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="H9" s="1">
         <v>45224</v>
       </c>
-      <c r="I9" s="1" t="n">
+      <c r="I9" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
-      <c r="B10"/>
       <c r="C10" t="s">
         <v>45</v>
       </c>
       <c r="D10" t="s">
         <v>45</v>
       </c>
-      <c r="E10"/>
       <c r="F10" t="s">
         <v>46</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10">
         <v>874940</v>
       </c>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="1">
         <v>45035</v>
       </c>
-      <c r="I10" s="1" t="n">
+      <c r="I10" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -1007,23 +1043,23 @@
       <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11">
         <v>150829</v>
       </c>
       <c r="F11" t="s">
         <v>51</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11">
         <v>263000</v>
       </c>
-      <c r="H11" s="1" t="n">
+      <c r="H11" s="1">
         <v>45035</v>
       </c>
-      <c r="I11" s="1" t="n">
+      <c r="I11" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>52</v>
       </c>
@@ -1036,23 +1072,23 @@
       <c r="D12" t="s">
         <v>54</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12">
         <v>150978</v>
       </c>
       <c r="F12" t="s">
         <v>55</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12">
         <v>195000</v>
       </c>
-      <c r="H12" s="1" t="n">
+      <c r="H12" s="1">
         <v>44846</v>
       </c>
-      <c r="I12" s="1" t="n">
+      <c r="I12" s="1">
         <v>45058</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1065,23 +1101,23 @@
       <c r="D13" t="s">
         <v>58</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13">
         <v>151293</v>
       </c>
       <c r="F13" t="s">
         <v>59</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13">
         <v>172860</v>
       </c>
-      <c r="H13" s="1" t="n">
+      <c r="H13" s="1">
         <v>44859</v>
       </c>
-      <c r="I13" s="1" t="n">
+      <c r="I13" s="1">
         <v>45071</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1094,23 +1130,23 @@
       <c r="D14" t="s">
         <v>63</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14">
         <v>191303</v>
       </c>
       <c r="F14" t="s">
         <v>64</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14">
         <v>449850</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="H14" s="1">
         <v>45119</v>
       </c>
-      <c r="I14" s="1" t="n">
+      <c r="I14" s="1">
         <v>45626</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>65</v>
       </c>
@@ -1123,23 +1159,23 @@
       <c r="D15" t="s">
         <v>68</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15">
         <v>150853</v>
       </c>
       <c r="F15" t="s">
         <v>69</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15">
         <v>205000</v>
       </c>
-      <c r="H15" s="1" t="n">
+      <c r="H15" s="1">
         <v>45247</v>
       </c>
-      <c r="I15" s="1" t="n">
+      <c r="I15" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>70</v>
       </c>
@@ -1152,23 +1188,23 @@
       <c r="D16" t="s">
         <v>73</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16">
         <v>151273</v>
       </c>
       <c r="F16" t="s">
         <v>74</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16">
         <v>349875</v>
       </c>
-      <c r="H16" s="1" t="n">
+      <c r="H16" s="1">
         <v>45205</v>
       </c>
-      <c r="I16" s="1" t="n">
+      <c r="I16" s="1">
         <v>45535</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>75</v>
       </c>
@@ -1181,23 +1217,23 @@
       <c r="D17" t="s">
         <v>78</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17">
         <v>150977</v>
       </c>
       <c r="F17" t="s">
         <v>79</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17">
         <v>1056672.77</v>
       </c>
-      <c r="H17" s="1" t="n">
+      <c r="H17" s="1">
         <v>45034</v>
       </c>
-      <c r="I17" s="1" t="n">
+      <c r="I17" s="1">
         <v>45473</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>80</v>
       </c>
@@ -1210,23 +1246,23 @@
       <c r="D18" t="s">
         <v>83</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18">
         <v>150981</v>
       </c>
       <c r="F18" t="s">
         <v>84</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18">
         <v>180000</v>
       </c>
-      <c r="H18" s="1" t="n">
+      <c r="H18" s="1">
         <v>45035</v>
       </c>
-      <c r="I18" s="1" t="n">
+      <c r="I18" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -1239,23 +1275,23 @@
       <c r="D19" t="s">
         <v>87</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19">
         <v>150983</v>
       </c>
       <c r="F19" t="s">
         <v>88</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19">
         <v>200000</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="H19" s="1">
         <v>44855</v>
       </c>
-      <c r="I19" s="1" t="n">
+      <c r="I19" s="1">
         <v>45067</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>85</v>
       </c>
@@ -1268,23 +1304,23 @@
       <c r="D20" t="s">
         <v>87</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20">
         <v>150983</v>
       </c>
       <c r="F20" t="s">
         <v>89</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20">
         <v>668400</v>
       </c>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="1">
         <v>45146</v>
       </c>
-      <c r="I20" s="1" t="n">
+      <c r="I20" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -1297,23 +1333,23 @@
       <c r="D21" t="s">
         <v>92</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21">
         <v>151276</v>
       </c>
       <c r="F21" t="s">
         <v>93</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21">
         <v>1557468.48</v>
       </c>
-      <c r="H21" s="1" t="n">
+      <c r="H21" s="1">
         <v>45084</v>
       </c>
-      <c r="I21" s="1" t="n">
+      <c r="I21" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>94</v>
       </c>
@@ -1326,23 +1362,23 @@
       <c r="D22" t="s">
         <v>96</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22">
         <v>150828</v>
       </c>
       <c r="F22" t="s">
         <v>97</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22">
         <v>455000</v>
       </c>
-      <c r="H22" s="1" t="n">
+      <c r="H22" s="1">
         <v>45183</v>
       </c>
-      <c r="I22" s="1" t="n">
+      <c r="I22" s="1">
         <v>45473</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>98</v>
       </c>
@@ -1355,23 +1391,23 @@
       <c r="D23" t="s">
         <v>101</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23">
         <v>150988</v>
       </c>
       <c r="F23" t="s">
         <v>102</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23">
         <v>454350</v>
       </c>
-      <c r="H23" s="1" t="n">
+      <c r="H23" s="1">
         <v>45218</v>
       </c>
-      <c r="I23" s="1" t="n">
+      <c r="I23" s="1">
         <v>45657</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>103</v>
       </c>
@@ -1384,23 +1420,23 @@
       <c r="D24" t="s">
         <v>106</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24">
         <v>151272</v>
       </c>
       <c r="F24" t="s">
         <v>107</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24">
         <v>99060</v>
       </c>
-      <c r="H24" s="1" t="n">
+      <c r="H24" s="1">
         <v>45205</v>
       </c>
-      <c r="I24" s="1" t="n">
+      <c r="I24" s="1">
         <v>45291</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>108</v>
       </c>
@@ -1413,23 +1449,23 @@
       <c r="D25" t="s">
         <v>111</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25">
         <v>151251</v>
       </c>
       <c r="F25" t="s">
         <v>112</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25">
         <v>152000</v>
       </c>
-      <c r="H25" s="1" t="n">
+      <c r="H25" s="1">
         <v>45209</v>
       </c>
-      <c r="I25" s="1" t="n">
+      <c r="I25" s="1">
         <v>45535</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>113</v>
       </c>
@@ -1439,27 +1475,32 @@
       <c r="C26" t="s">
         <v>115</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26">
         <v>150822</v>
       </c>
       <c r="F26" t="s">
         <v>117</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26">
         <v>200000</v>
       </c>
-      <c r="H26" s="1" t="n">
+      <c r="H26" s="1">
         <v>44886</v>
       </c>
-      <c r="I26" s="1" t="n">
+      <c r="I26" s="1">
         <v>45098</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D8" r:id="rId1" xr:uid="{F78DFE50-675E-E746-B229-C7578CD71FEB}"/>
+    <hyperlink ref="D26" r:id="rId2" xr:uid="{798B476E-A932-6D4A-9CA1-1B5A537BC374}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{9C977226-6AA7-8B42-88E6-29E83D294F08}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>